<commit_message>
Major changes to MS over the past two weeks prior to resubmission
</commit_message>
<xml_diff>
--- a/Review_Spreadsheet.xlsx
+++ b/Review_Spreadsheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saoirsekelleher/Documents/Research/QAEco/DOM_Review/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE75479-CD29-DD4C-A432-289D9DA46A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1615C13A-932A-E245-ADEB-950A768A9AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16620" yWindow="2680" windowWidth="35540" windowHeight="23940" activeTab="1" xr2:uid="{981D9C2C-D510-E947-BD55-27C976277DB6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="4" xr2:uid="{981D9C2C-D510-E947-BD55-27C976277DB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Article Data" sheetId="10" r:id="rId1"/>
@@ -6196,27 +6196,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6224,6 +6203,147 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6245,126 +6365,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -9122,9 +9122,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02CC6A4-A2FF-2943-B085-9BDC0511411B}">
   <dimension ref="A1:I130"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A94" sqref="A94:I111"/>
+      <selection pane="bottomLeft" activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -19673,9 +19673,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60FD29C-9206-FA47-9E36-5CC91A5A2C02}">
   <dimension ref="A1:Q211"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -26803,7 +26803,7 @@
         <v>41426</v>
       </c>
       <c r="F130" s="39">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="G130" s="39">
         <v>3</v>
@@ -34499,7 +34499,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="286" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A286" s="38">
         <f>'Article Data'!A65</f>
         <v>488</v>
@@ -34524,7 +34524,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="287" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A287" s="39">
         <f>'Article Data'!A65</f>
         <v>488</v>
@@ -34549,7 +34549,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="288" spans="1:7" ht="409.5" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A288" s="38">
         <f>'Article Data'!A65</f>
         <v>488</v>
@@ -42116,13 +42116,13 @@
   <sheetData>
     <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
-      <c r="B1" s="90" t="s">
+      <c r="B1" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="90"/>
-      <c r="D1" s="90"/>
-      <c r="E1" s="90"/>
-      <c r="F1" s="90"/>
+      <c r="C1" s="78"/>
+      <c r="D1" s="78"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="78"/>
     </row>
     <row r="2" spans="1:6" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -42145,7 +42145,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="95" t="s">
+      <c r="A3" s="80" t="s">
         <v>290</v>
       </c>
       <c r="B3" s="23" t="s">
@@ -42161,7 +42161,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="96"/>
+      <c r="A4" s="81"/>
       <c r="B4" s="23" t="s">
         <v>2</v>
       </c>
@@ -42175,7 +42175,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="96"/>
+      <c r="A5" s="81"/>
       <c r="B5" s="23" t="s">
         <v>13</v>
       </c>
@@ -42191,7 +42191,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A6" s="97"/>
+      <c r="A6" s="82"/>
       <c r="B6" s="23" t="s">
         <v>14</v>
       </c>
@@ -42207,7 +42207,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="99" t="s">
+      <c r="A7" s="84" t="s">
         <v>47</v>
       </c>
       <c r="B7" s="24" t="s">
@@ -42223,14 +42223,14 @@
       <c r="F7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="99"/>
-      <c r="B8" s="98" t="s">
+      <c r="A8" s="84"/>
+      <c r="B8" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="109" t="s">
+      <c r="C8" s="68" t="s">
         <v>1047</v>
       </c>
-      <c r="D8" s="110" t="s">
+      <c r="D8" s="69" t="s">
         <v>48</v>
       </c>
       <c r="E8" s="9" t="s">
@@ -42241,10 +42241,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="99"/>
-      <c r="B9" s="98"/>
-      <c r="C9" s="109"/>
-      <c r="D9" s="110"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="83"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="69"/>
       <c r="E9" s="9" t="s">
         <v>342</v>
       </c>
@@ -42253,10 +42253,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="99"/>
-      <c r="B10" s="98"/>
-      <c r="C10" s="109"/>
-      <c r="D10" s="110"/>
+      <c r="A10" s="84"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="69"/>
       <c r="E10" s="9" t="s">
         <v>343</v>
       </c>
@@ -42265,10 +42265,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="99"/>
-      <c r="B11" s="98"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="110"/>
+      <c r="A11" s="84"/>
+      <c r="B11" s="83"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="69"/>
       <c r="E11" s="9" t="s">
         <v>344</v>
       </c>
@@ -42277,10 +42277,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="99"/>
-      <c r="B12" s="98"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="110"/>
+      <c r="A12" s="84"/>
+      <c r="B12" s="83"/>
+      <c r="C12" s="68"/>
+      <c r="D12" s="69"/>
       <c r="E12" s="9" t="s">
         <v>345</v>
       </c>
@@ -42289,7 +42289,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="99"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="24" t="s">
         <v>5</v>
       </c>
@@ -42303,7 +42303,7 @@
       <c r="F13" s="9"/>
     </row>
     <row r="14" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="99"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="24" t="s">
         <v>6</v>
       </c>
@@ -42317,7 +42317,7 @@
       <c r="F14" s="9"/>
     </row>
     <row r="15" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A15" s="99"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="24" t="s">
         <v>1026</v>
       </c>
@@ -42333,16 +42333,16 @@
       <c r="F15" s="9"/>
     </row>
     <row r="16" spans="1:6" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="106" t="s">
+      <c r="A16" s="88" t="s">
         <v>309</v>
       </c>
-      <c r="B16" s="103" t="s">
+      <c r="B16" s="85" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="100" t="s">
+      <c r="C16" s="70" t="s">
         <v>1027</v>
       </c>
-      <c r="D16" s="100" t="s">
+      <c r="D16" s="70" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="30" t="s">
@@ -42353,10 +42353,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="107"/>
-      <c r="B17" s="104"/>
-      <c r="C17" s="101"/>
-      <c r="D17" s="101"/>
+      <c r="A17" s="89"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="71"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="30" t="s">
         <v>311</v>
       </c>
@@ -42365,10 +42365,10 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="107"/>
-      <c r="B18" s="104"/>
-      <c r="C18" s="101"/>
-      <c r="D18" s="101"/>
+      <c r="A18" s="89"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="71"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="30" t="s">
         <v>312</v>
       </c>
@@ -42377,10 +42377,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="107"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="102"/>
-      <c r="D19" s="102"/>
+      <c r="A19" s="89"/>
+      <c r="B19" s="87"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="30" t="s">
         <v>313</v>
       </c>
@@ -42389,7 +42389,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A20" s="107"/>
+      <c r="A20" s="89"/>
       <c r="B20" s="31" t="s">
         <v>8</v>
       </c>
@@ -42403,7 +42403,7 @@
       <c r="F20" s="30"/>
     </row>
     <row r="21" spans="1:6" ht="85" x14ac:dyDescent="0.2">
-      <c r="A21" s="107"/>
+      <c r="A21" s="89"/>
       <c r="B21" s="31" t="s">
         <v>1028</v>
       </c>
@@ -42417,7 +42417,7 @@
       <c r="F21" s="30"/>
     </row>
     <row r="22" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A22" s="107"/>
+      <c r="A22" s="89"/>
       <c r="B22" s="31" t="s">
         <v>9</v>
       </c>
@@ -42431,7 +42431,7 @@
       <c r="F22" s="30"/>
     </row>
     <row r="23" spans="1:6" ht="51" x14ac:dyDescent="0.2">
-      <c r="A23" s="107"/>
+      <c r="A23" s="89"/>
       <c r="B23" s="31" t="s">
         <v>10</v>
       </c>
@@ -42445,7 +42445,7 @@
       <c r="F23" s="30"/>
     </row>
     <row r="24" spans="1:6" ht="34" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="107"/>
+      <c r="A24" s="89"/>
       <c r="B24" s="31" t="s">
         <v>11</v>
       </c>
@@ -42459,7 +42459,7 @@
       <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A25" s="107"/>
+      <c r="A25" s="89"/>
       <c r="B25" s="31" t="s">
         <v>11</v>
       </c>
@@ -42473,7 +42473,7 @@
       <c r="F25" s="30"/>
     </row>
     <row r="26" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="108"/>
+      <c r="A26" s="90"/>
       <c r="B26" s="31" t="s">
         <v>12</v>
       </c>
@@ -42487,7 +42487,7 @@
       <c r="F26" s="30"/>
     </row>
     <row r="27" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="91" t="s">
+      <c r="A27" s="79" t="s">
         <v>308</v>
       </c>
       <c r="B27" s="25" t="s">
@@ -42503,14 +42503,14 @@
       <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28" s="91"/>
-      <c r="B28" s="94" t="s">
+      <c r="A28" s="79"/>
+      <c r="B28" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="93" t="s">
+      <c r="C28" s="66" t="s">
         <v>1041</v>
       </c>
-      <c r="D28" s="92" t="s">
+      <c r="D28" s="65" t="s">
         <v>53</v>
       </c>
       <c r="E28" s="12" t="s">
@@ -42521,10 +42521,10 @@
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="91"/>
-      <c r="B29" s="94"/>
-      <c r="C29" s="93"/>
-      <c r="D29" s="92"/>
+      <c r="A29" s="79"/>
+      <c r="B29" s="60"/>
+      <c r="C29" s="66"/>
+      <c r="D29" s="65"/>
       <c r="E29" s="12" t="s">
         <v>55</v>
       </c>
@@ -42533,10 +42533,10 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30" s="91"/>
-      <c r="B30" s="94"/>
-      <c r="C30" s="93"/>
-      <c r="D30" s="92"/>
+      <c r="A30" s="79"/>
+      <c r="B30" s="60"/>
+      <c r="C30" s="66"/>
+      <c r="D30" s="65"/>
       <c r="E30" s="12" t="s">
         <v>56</v>
       </c>
@@ -42545,10 +42545,10 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="91"/>
-      <c r="B31" s="94"/>
-      <c r="C31" s="93"/>
-      <c r="D31" s="92"/>
+      <c r="A31" s="79"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="66"/>
+      <c r="D31" s="65"/>
       <c r="E31" s="12" t="s">
         <v>59</v>
       </c>
@@ -42557,10 +42557,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="91"/>
-      <c r="B32" s="94"/>
-      <c r="C32" s="93"/>
-      <c r="D32" s="92"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="65"/>
       <c r="E32" s="12" t="s">
         <v>58</v>
       </c>
@@ -42569,10 +42569,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="91"/>
-      <c r="B33" s="94"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="92"/>
+      <c r="A33" s="79"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="66"/>
+      <c r="D33" s="65"/>
       <c r="E33" s="12" t="s">
         <v>57</v>
       </c>
@@ -42581,7 +42581,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="68" x14ac:dyDescent="0.2">
-      <c r="A34" s="91"/>
+      <c r="A34" s="79"/>
       <c r="B34" s="25" t="s">
         <v>18</v>
       </c>
@@ -42595,14 +42595,14 @@
       <c r="F34" s="12"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35" s="91"/>
-      <c r="B35" s="94" t="s">
+      <c r="A35" s="79"/>
+      <c r="B35" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="93" t="s">
+      <c r="C35" s="66" t="s">
         <v>1036</v>
       </c>
-      <c r="D35" s="92" t="s">
+      <c r="D35" s="65" t="s">
         <v>48</v>
       </c>
       <c r="E35" s="12" t="s">
@@ -42613,10 +42613,10 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36" s="91"/>
-      <c r="B36" s="94"/>
-      <c r="C36" s="93"/>
-      <c r="D36" s="92"/>
+      <c r="A36" s="79"/>
+      <c r="B36" s="60"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="65"/>
       <c r="E36" s="12" t="s">
         <v>67</v>
       </c>
@@ -42625,10 +42625,10 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37" s="91"/>
-      <c r="B37" s="94"/>
-      <c r="C37" s="93"/>
-      <c r="D37" s="92"/>
+      <c r="A37" s="79"/>
+      <c r="B37" s="60"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="65"/>
       <c r="E37" s="12" t="s">
         <v>70</v>
       </c>
@@ -42637,10 +42637,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38" s="91"/>
-      <c r="B38" s="94"/>
-      <c r="C38" s="93"/>
-      <c r="D38" s="92"/>
+      <c r="A38" s="79"/>
+      <c r="B38" s="60"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="65"/>
       <c r="E38" s="12" t="s">
         <v>72</v>
       </c>
@@ -42649,14 +42649,14 @@
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39" s="91"/>
-      <c r="B39" s="94" t="s">
+      <c r="A39" s="79"/>
+      <c r="B39" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="93" t="s">
+      <c r="C39" s="66" t="s">
         <v>1040</v>
       </c>
-      <c r="D39" s="92" t="s">
+      <c r="D39" s="65" t="s">
         <v>53</v>
       </c>
       <c r="E39" s="12" t="s">
@@ -42667,10 +42667,10 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="91"/>
-      <c r="B40" s="94"/>
-      <c r="C40" s="93"/>
-      <c r="D40" s="92"/>
+      <c r="A40" s="79"/>
+      <c r="B40" s="60"/>
+      <c r="C40" s="66"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="12" t="s">
         <v>74</v>
       </c>
@@ -42679,10 +42679,10 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="91"/>
-      <c r="B41" s="94"/>
-      <c r="C41" s="93"/>
-      <c r="D41" s="92"/>
+      <c r="A41" s="79"/>
+      <c r="B41" s="60"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="65"/>
       <c r="E41" s="12" t="s">
         <v>76</v>
       </c>
@@ -42691,10 +42691,10 @@
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42" s="91"/>
-      <c r="B42" s="94"/>
-      <c r="C42" s="93"/>
-      <c r="D42" s="92"/>
+      <c r="A42" s="79"/>
+      <c r="B42" s="60"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="65"/>
       <c r="E42" s="12" t="s">
         <v>338</v>
       </c>
@@ -42703,10 +42703,10 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="91"/>
-      <c r="B43" s="94"/>
-      <c r="C43" s="93"/>
-      <c r="D43" s="92"/>
+      <c r="A43" s="79"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="65"/>
       <c r="E43" s="12" t="s">
         <v>77</v>
       </c>
@@ -42715,10 +42715,10 @@
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44" s="91"/>
-      <c r="B44" s="94"/>
-      <c r="C44" s="93"/>
-      <c r="D44" s="92"/>
+      <c r="A44" s="79"/>
+      <c r="B44" s="60"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="65"/>
       <c r="E44" s="12" t="s">
         <v>78</v>
       </c>
@@ -42727,10 +42727,10 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="91"/>
-      <c r="B45" s="94"/>
-      <c r="C45" s="93"/>
-      <c r="D45" s="92"/>
+      <c r="A45" s="79"/>
+      <c r="B45" s="60"/>
+      <c r="C45" s="66"/>
+      <c r="D45" s="65"/>
       <c r="E45" s="12" t="s">
         <v>79</v>
       </c>
@@ -42739,10 +42739,10 @@
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A46" s="91"/>
-      <c r="B46" s="94"/>
-      <c r="C46" s="93"/>
-      <c r="D46" s="92"/>
+      <c r="A46" s="79"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="66"/>
+      <c r="D46" s="65"/>
       <c r="E46" s="12" t="s">
         <v>80</v>
       </c>
@@ -42751,10 +42751,10 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="91"/>
-      <c r="B47" s="94"/>
-      <c r="C47" s="93"/>
-      <c r="D47" s="92"/>
+      <c r="A47" s="79"/>
+      <c r="B47" s="60"/>
+      <c r="C47" s="66"/>
+      <c r="D47" s="65"/>
       <c r="E47" s="12" t="s">
         <v>81</v>
       </c>
@@ -42763,14 +42763,14 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="91"/>
-      <c r="B48" s="94" t="s">
+      <c r="A48" s="79"/>
+      <c r="B48" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C48" s="93" t="s">
+      <c r="C48" s="66" t="s">
         <v>1039</v>
       </c>
-      <c r="D48" s="92" t="s">
+      <c r="D48" s="65" t="s">
         <v>53</v>
       </c>
       <c r="E48" s="12" t="s">
@@ -42781,10 +42781,10 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="91"/>
-      <c r="B49" s="94"/>
-      <c r="C49" s="93"/>
-      <c r="D49" s="92"/>
+      <c r="A49" s="79"/>
+      <c r="B49" s="60"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="65"/>
       <c r="E49" s="12" t="s">
         <v>92</v>
       </c>
@@ -42793,10 +42793,10 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="91"/>
-      <c r="B50" s="94"/>
-      <c r="C50" s="93"/>
-      <c r="D50" s="92"/>
+      <c r="A50" s="79"/>
+      <c r="B50" s="60"/>
+      <c r="C50" s="66"/>
+      <c r="D50" s="65"/>
       <c r="E50" s="12" t="s">
         <v>93</v>
       </c>
@@ -42805,10 +42805,10 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="91"/>
-      <c r="B51" s="94"/>
-      <c r="C51" s="93"/>
-      <c r="D51" s="92"/>
+      <c r="A51" s="79"/>
+      <c r="B51" s="60"/>
+      <c r="C51" s="66"/>
+      <c r="D51" s="65"/>
       <c r="E51" s="12" t="s">
         <v>94</v>
       </c>
@@ -42817,10 +42817,10 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="91"/>
-      <c r="B52" s="94"/>
-      <c r="C52" s="93"/>
-      <c r="D52" s="92"/>
+      <c r="A52" s="79"/>
+      <c r="B52" s="60"/>
+      <c r="C52" s="66"/>
+      <c r="D52" s="65"/>
       <c r="E52" s="12" t="s">
         <v>95</v>
       </c>
@@ -42829,10 +42829,10 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="91"/>
-      <c r="B53" s="94"/>
-      <c r="C53" s="93"/>
-      <c r="D53" s="92"/>
+      <c r="A53" s="79"/>
+      <c r="B53" s="60"/>
+      <c r="C53" s="66"/>
+      <c r="D53" s="65"/>
       <c r="E53" s="12" t="s">
         <v>97</v>
       </c>
@@ -42841,10 +42841,10 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="91"/>
-      <c r="B54" s="94"/>
-      <c r="C54" s="93"/>
-      <c r="D54" s="92"/>
+      <c r="A54" s="79"/>
+      <c r="B54" s="60"/>
+      <c r="C54" s="66"/>
+      <c r="D54" s="65"/>
       <c r="E54" s="12" t="s">
         <v>57</v>
       </c>
@@ -42853,10 +42853,10 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="91"/>
-      <c r="B55" s="94"/>
-      <c r="C55" s="93"/>
-      <c r="D55" s="92"/>
+      <c r="A55" s="79"/>
+      <c r="B55" s="60"/>
+      <c r="C55" s="66"/>
+      <c r="D55" s="65"/>
       <c r="E55" s="12" t="s">
         <v>96</v>
       </c>
@@ -42865,10 +42865,10 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="91"/>
-      <c r="B56" s="94"/>
-      <c r="C56" s="93"/>
-      <c r="D56" s="92"/>
+      <c r="A56" s="79"/>
+      <c r="B56" s="60"/>
+      <c r="C56" s="66"/>
+      <c r="D56" s="65"/>
       <c r="E56" s="12" t="s">
         <v>81</v>
       </c>
@@ -42877,7 +42877,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="72" t="s">
+      <c r="A57" s="97" t="s">
         <v>107</v>
       </c>
       <c r="B57" s="28" t="s">
@@ -42895,14 +42895,14 @@
       <c r="F57" s="13"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="73"/>
-      <c r="B58" s="82" t="s">
+      <c r="A58" s="98"/>
+      <c r="B58" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="C58" s="81" t="s">
+      <c r="C58" s="92" t="s">
         <v>1037</v>
       </c>
-      <c r="D58" s="84" t="s">
+      <c r="D58" s="64" t="s">
         <v>48</v>
       </c>
       <c r="E58" s="13" t="s">
@@ -42911,132 +42911,132 @@
       <c r="F58" s="13"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="73"/>
-      <c r="B59" s="82"/>
-      <c r="C59" s="81"/>
-      <c r="D59" s="84"/>
+      <c r="A59" s="98"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="92"/>
+      <c r="D59" s="64"/>
       <c r="E59" s="13" t="s">
         <v>111</v>
       </c>
       <c r="F59" s="13"/>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="73"/>
-      <c r="B60" s="82"/>
-      <c r="C60" s="81"/>
-      <c r="D60" s="84"/>
+      <c r="A60" s="98"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="92"/>
+      <c r="D60" s="64"/>
       <c r="E60" s="13" t="s">
         <v>110</v>
       </c>
       <c r="F60" s="13"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="73"/>
-      <c r="B61" s="82"/>
-      <c r="C61" s="81"/>
-      <c r="D61" s="84"/>
+      <c r="A61" s="98"/>
+      <c r="B61" s="93"/>
+      <c r="C61" s="92"/>
+      <c r="D61" s="64"/>
       <c r="E61" s="13" t="s">
         <v>108</v>
       </c>
       <c r="F61" s="13"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="73"/>
-      <c r="B62" s="82"/>
-      <c r="C62" s="81"/>
-      <c r="D62" s="84"/>
+      <c r="A62" s="98"/>
+      <c r="B62" s="93"/>
+      <c r="C62" s="92"/>
+      <c r="D62" s="64"/>
       <c r="E62" s="13" t="s">
         <v>113</v>
       </c>
       <c r="F62" s="13"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="73"/>
-      <c r="B63" s="82"/>
-      <c r="C63" s="81"/>
-      <c r="D63" s="84"/>
+      <c r="A63" s="98"/>
+      <c r="B63" s="93"/>
+      <c r="C63" s="92"/>
+      <c r="D63" s="64"/>
       <c r="E63" s="13" t="s">
         <v>109</v>
       </c>
       <c r="F63" s="13"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="73"/>
-      <c r="B64" s="82" t="s">
+      <c r="A64" s="98"/>
+      <c r="B64" s="93" t="s">
         <v>21</v>
       </c>
-      <c r="C64" s="81" t="s">
+      <c r="C64" s="92" t="s">
         <v>1025</v>
       </c>
-      <c r="D64" s="84" t="s">
+      <c r="D64" s="64" t="s">
         <v>48</v>
       </c>
       <c r="E64" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="F64" s="83" t="e" vm="1">
+      <c r="F64" s="91" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="73"/>
-      <c r="B65" s="82"/>
-      <c r="C65" s="81"/>
-      <c r="D65" s="84"/>
+      <c r="A65" s="98"/>
+      <c r="B65" s="93"/>
+      <c r="C65" s="92"/>
+      <c r="D65" s="64"/>
       <c r="E65" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F65" s="83"/>
+      <c r="F65" s="91"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="73"/>
-      <c r="B66" s="82"/>
-      <c r="C66" s="81"/>
-      <c r="D66" s="84"/>
+      <c r="A66" s="98"/>
+      <c r="B66" s="93"/>
+      <c r="C66" s="92"/>
+      <c r="D66" s="64"/>
       <c r="E66" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="F66" s="83"/>
+      <c r="F66" s="91"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="73"/>
-      <c r="B67" s="82"/>
-      <c r="C67" s="81"/>
-      <c r="D67" s="84"/>
+      <c r="A67" s="98"/>
+      <c r="B67" s="93"/>
+      <c r="C67" s="92"/>
+      <c r="D67" s="64"/>
       <c r="E67" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="F67" s="83"/>
+      <c r="F67" s="91"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="73"/>
-      <c r="B68" s="82"/>
-      <c r="C68" s="81"/>
-      <c r="D68" s="84"/>
+      <c r="A68" s="98"/>
+      <c r="B68" s="93"/>
+      <c r="C68" s="92"/>
+      <c r="D68" s="64"/>
       <c r="E68" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="F68" s="83"/>
+      <c r="F68" s="91"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="73"/>
-      <c r="B69" s="82"/>
-      <c r="C69" s="81"/>
-      <c r="D69" s="84"/>
+      <c r="A69" s="98"/>
+      <c r="B69" s="93"/>
+      <c r="C69" s="92"/>
+      <c r="D69" s="64"/>
       <c r="E69" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F69" s="83"/>
+      <c r="F69" s="91"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="73"/>
-      <c r="B70" s="82" t="s">
+      <c r="A70" s="98"/>
+      <c r="B70" s="93" t="s">
         <v>22</v>
       </c>
-      <c r="C70" s="81" t="s">
+      <c r="C70" s="92" t="s">
         <v>1024</v>
       </c>
-      <c r="D70" s="84" t="s">
+      <c r="D70" s="64" t="s">
         <v>48</v>
       </c>
       <c r="E70" s="13" t="s">
@@ -43045,87 +43045,87 @@
       <c r="F70" s="13"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="73"/>
-      <c r="B71" s="82"/>
-      <c r="C71" s="81"/>
-      <c r="D71" s="84"/>
+      <c r="A71" s="98"/>
+      <c r="B71" s="93"/>
+      <c r="C71" s="92"/>
+      <c r="D71" s="64"/>
       <c r="E71" s="15" t="s">
         <v>120</v>
       </c>
       <c r="F71" s="13"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="73"/>
-      <c r="B72" s="82"/>
-      <c r="C72" s="81"/>
-      <c r="D72" s="84"/>
+      <c r="A72" s="98"/>
+      <c r="B72" s="93"/>
+      <c r="C72" s="92"/>
+      <c r="D72" s="64"/>
       <c r="E72" s="13" t="s">
         <v>121</v>
       </c>
       <c r="F72" s="13"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="73"/>
-      <c r="B73" s="82"/>
-      <c r="C73" s="81"/>
-      <c r="D73" s="84"/>
+      <c r="A73" s="98"/>
+      <c r="B73" s="93"/>
+      <c r="C73" s="92"/>
+      <c r="D73" s="64"/>
       <c r="E73" s="13" t="s">
         <v>122</v>
       </c>
       <c r="F73" s="13"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="73"/>
-      <c r="B74" s="82"/>
-      <c r="C74" s="81"/>
-      <c r="D74" s="84"/>
+      <c r="A74" s="98"/>
+      <c r="B74" s="93"/>
+      <c r="C74" s="92"/>
+      <c r="D74" s="64"/>
       <c r="E74" s="13" t="s">
         <v>124</v>
       </c>
       <c r="F74" s="13"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="73"/>
-      <c r="B75" s="82"/>
-      <c r="C75" s="81"/>
-      <c r="D75" s="84"/>
+      <c r="A75" s="98"/>
+      <c r="B75" s="93"/>
+      <c r="C75" s="92"/>
+      <c r="D75" s="64"/>
       <c r="E75" s="13" t="s">
         <v>123</v>
       </c>
       <c r="F75" s="13"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="73"/>
-      <c r="B76" s="82"/>
-      <c r="C76" s="81"/>
-      <c r="D76" s="84"/>
+      <c r="A76" s="98"/>
+      <c r="B76" s="93"/>
+      <c r="C76" s="92"/>
+      <c r="D76" s="64"/>
       <c r="E76" s="13" t="s">
         <v>125</v>
       </c>
       <c r="F76" s="13"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="73"/>
-      <c r="B77" s="82"/>
-      <c r="C77" s="81"/>
-      <c r="D77" s="84"/>
+      <c r="A77" s="98"/>
+      <c r="B77" s="93"/>
+      <c r="C77" s="92"/>
+      <c r="D77" s="64"/>
       <c r="E77" s="13" t="s">
         <v>126</v>
       </c>
       <c r="F77" s="13"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="73"/>
-      <c r="B78" s="82"/>
-      <c r="C78" s="81"/>
-      <c r="D78" s="84"/>
+      <c r="A78" s="98"/>
+      <c r="B78" s="93"/>
+      <c r="C78" s="92"/>
+      <c r="D78" s="64"/>
       <c r="E78" s="13" t="s">
         <v>322</v>
       </c>
       <c r="F78" s="13"/>
     </row>
     <row r="79" spans="1:6" ht="136" x14ac:dyDescent="0.2">
-      <c r="A79" s="77" t="s">
+      <c r="A79" s="102" t="s">
         <v>127</v>
       </c>
       <c r="B79" s="26" t="s">
@@ -43141,7 +43141,7 @@
       <c r="F79" s="16"/>
     </row>
     <row r="80" spans="1:6" ht="119" x14ac:dyDescent="0.2">
-      <c r="A80" s="77"/>
+      <c r="A80" s="102"/>
       <c r="B80" s="26" t="s">
         <v>27</v>
       </c>
@@ -43155,7 +43155,7 @@
       <c r="F80" s="16"/>
     </row>
     <row r="81" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A81" s="77"/>
+      <c r="A81" s="102"/>
       <c r="B81" s="26" t="s">
         <v>23</v>
       </c>
@@ -43169,7 +43169,7 @@
       <c r="F81" s="16"/>
     </row>
     <row r="82" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A82" s="77"/>
+      <c r="A82" s="102"/>
       <c r="B82" s="26" t="s">
         <v>1052</v>
       </c>
@@ -43183,7 +43183,7 @@
       <c r="F82" s="16"/>
     </row>
     <row r="83" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A83" s="77"/>
+      <c r="A83" s="102"/>
       <c r="B83" s="53" t="s">
         <v>1054</v>
       </c>
@@ -43197,7 +43197,7 @@
       <c r="F83" s="16"/>
     </row>
     <row r="84" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A84" s="77"/>
+      <c r="A84" s="102"/>
       <c r="B84" s="53" t="s">
         <v>1055</v>
       </c>
@@ -43211,7 +43211,7 @@
       <c r="F84" s="16"/>
     </row>
     <row r="85" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A85" s="77"/>
+      <c r="A85" s="102"/>
       <c r="B85" s="53" t="s">
         <v>1056</v>
       </c>
@@ -43225,7 +43225,7 @@
       <c r="F85" s="16"/>
     </row>
     <row r="86" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A86" s="77"/>
+      <c r="A86" s="102"/>
       <c r="B86" s="53" t="s">
         <v>1057</v>
       </c>
@@ -43239,14 +43239,14 @@
       <c r="F86" s="16"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="77"/>
-      <c r="B87" s="76" t="s">
+      <c r="A87" s="102"/>
+      <c r="B87" s="101" t="s">
         <v>24</v>
       </c>
-      <c r="C87" s="75" t="s">
+      <c r="C87" s="100" t="s">
         <v>1062</v>
       </c>
-      <c r="D87" s="74" t="s">
+      <c r="D87" s="99" t="s">
         <v>48</v>
       </c>
       <c r="E87" s="16" t="s">
@@ -43257,10 +43257,10 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="77"/>
-      <c r="B88" s="76"/>
-      <c r="C88" s="75"/>
-      <c r="D88" s="74"/>
+      <c r="A88" s="102"/>
+      <c r="B88" s="101"/>
+      <c r="C88" s="100"/>
+      <c r="D88" s="99"/>
       <c r="E88" s="16" t="s">
         <v>320</v>
       </c>
@@ -43269,10 +43269,10 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="77"/>
-      <c r="B89" s="76"/>
-      <c r="C89" s="75"/>
-      <c r="D89" s="74"/>
+      <c r="A89" s="102"/>
+      <c r="B89" s="101"/>
+      <c r="C89" s="100"/>
+      <c r="D89" s="99"/>
       <c r="E89" s="16" t="s">
         <v>130</v>
       </c>
@@ -43281,10 +43281,10 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="77"/>
-      <c r="B90" s="76"/>
-      <c r="C90" s="75"/>
-      <c r="D90" s="74"/>
+      <c r="A90" s="102"/>
+      <c r="B90" s="101"/>
+      <c r="C90" s="100"/>
+      <c r="D90" s="99"/>
       <c r="E90" s="16" t="s">
         <v>131</v>
       </c>
@@ -43293,10 +43293,10 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="77"/>
-      <c r="B91" s="76"/>
-      <c r="C91" s="75"/>
-      <c r="D91" s="74"/>
+      <c r="A91" s="102"/>
+      <c r="B91" s="101"/>
+      <c r="C91" s="100"/>
+      <c r="D91" s="99"/>
       <c r="E91" s="16" t="s">
         <v>132</v>
       </c>
@@ -43305,10 +43305,10 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="77"/>
-      <c r="B92" s="76"/>
-      <c r="C92" s="75"/>
-      <c r="D92" s="74"/>
+      <c r="A92" s="102"/>
+      <c r="B92" s="101"/>
+      <c r="C92" s="100"/>
+      <c r="D92" s="99"/>
       <c r="E92" s="16" t="s">
         <v>137</v>
       </c>
@@ -43317,10 +43317,10 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="77"/>
-      <c r="B93" s="76"/>
-      <c r="C93" s="75"/>
-      <c r="D93" s="74"/>
+      <c r="A93" s="102"/>
+      <c r="B93" s="101"/>
+      <c r="C93" s="100"/>
+      <c r="D93" s="99"/>
       <c r="E93" s="16" t="s">
         <v>57</v>
       </c>
@@ -43329,10 +43329,10 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="77"/>
-      <c r="B94" s="76"/>
-      <c r="C94" s="75"/>
-      <c r="D94" s="74"/>
+      <c r="A94" s="102"/>
+      <c r="B94" s="101"/>
+      <c r="C94" s="100"/>
+      <c r="D94" s="99"/>
       <c r="E94" s="16" t="s">
         <v>133</v>
       </c>
@@ -43341,14 +43341,14 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="77"/>
-      <c r="B95" s="76" t="s">
+      <c r="A95" s="102"/>
+      <c r="B95" s="101" t="s">
         <v>26</v>
       </c>
-      <c r="C95" s="78" t="s">
+      <c r="C95" s="61" t="s">
         <v>1063</v>
       </c>
-      <c r="D95" s="78" t="s">
+      <c r="D95" s="61" t="s">
         <v>53</v>
       </c>
       <c r="E95" s="16" t="s">
@@ -43359,10 +43359,10 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="77"/>
-      <c r="B96" s="76"/>
-      <c r="C96" s="79"/>
-      <c r="D96" s="79"/>
+      <c r="A96" s="102"/>
+      <c r="B96" s="101"/>
+      <c r="C96" s="62"/>
+      <c r="D96" s="62"/>
       <c r="E96" s="16" t="s">
         <v>142</v>
       </c>
@@ -43371,10 +43371,10 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="77"/>
-      <c r="B97" s="76"/>
-      <c r="C97" s="79"/>
-      <c r="D97" s="79"/>
+      <c r="A97" s="102"/>
+      <c r="B97" s="101"/>
+      <c r="C97" s="62"/>
+      <c r="D97" s="62"/>
       <c r="E97" s="16" t="s">
         <v>144</v>
       </c>
@@ -43383,10 +43383,10 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A98" s="77"/>
-      <c r="B98" s="76"/>
-      <c r="C98" s="80"/>
-      <c r="D98" s="80"/>
+      <c r="A98" s="102"/>
+      <c r="B98" s="101"/>
+      <c r="C98" s="63"/>
+      <c r="D98" s="63"/>
       <c r="E98" s="16" t="s">
         <v>145</v>
       </c>
@@ -43395,7 +43395,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A99" s="77"/>
+      <c r="A99" s="102"/>
       <c r="B99" s="26" t="s">
         <v>150</v>
       </c>
@@ -43409,7 +43409,7 @@
       <c r="F99" s="16"/>
     </row>
     <row r="100" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A100" s="77"/>
+      <c r="A100" s="102"/>
       <c r="B100" s="26" t="s">
         <v>149</v>
       </c>
@@ -43423,14 +43423,14 @@
       <c r="F100" s="16"/>
     </row>
     <row r="101" spans="1:6" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="77"/>
-      <c r="B101" s="76" t="s">
+      <c r="A101" s="102"/>
+      <c r="B101" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="C101" s="75" t="s">
+      <c r="C101" s="100" t="s">
         <v>1065</v>
       </c>
-      <c r="D101" s="74" t="s">
+      <c r="D101" s="99" t="s">
         <v>48</v>
       </c>
       <c r="E101" s="16" t="s">
@@ -43441,10 +43441,10 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A102" s="77"/>
-      <c r="B102" s="76"/>
-      <c r="C102" s="75"/>
-      <c r="D102" s="74"/>
+      <c r="A102" s="102"/>
+      <c r="B102" s="101"/>
+      <c r="C102" s="100"/>
+      <c r="D102" s="99"/>
       <c r="E102" s="16" t="s">
         <v>154</v>
       </c>
@@ -43453,10 +43453,10 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A103" s="77"/>
-      <c r="B103" s="76"/>
-      <c r="C103" s="75"/>
-      <c r="D103" s="74"/>
+      <c r="A103" s="102"/>
+      <c r="B103" s="101"/>
+      <c r="C103" s="100"/>
+      <c r="D103" s="99"/>
       <c r="E103" s="16" t="s">
         <v>155</v>
       </c>
@@ -43465,10 +43465,10 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A104" s="77"/>
-      <c r="B104" s="76"/>
-      <c r="C104" s="75"/>
-      <c r="D104" s="74"/>
+      <c r="A104" s="102"/>
+      <c r="B104" s="101"/>
+      <c r="C104" s="100"/>
+      <c r="D104" s="99"/>
       <c r="E104" s="16" t="s">
         <v>330</v>
       </c>
@@ -43477,10 +43477,10 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A105" s="77"/>
-      <c r="B105" s="76"/>
-      <c r="C105" s="75"/>
-      <c r="D105" s="74"/>
+      <c r="A105" s="102"/>
+      <c r="B105" s="101"/>
+      <c r="C105" s="100"/>
+      <c r="D105" s="99"/>
       <c r="E105" s="16" t="s">
         <v>57</v>
       </c>
@@ -43489,14 +43489,14 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A106" s="77"/>
-      <c r="B106" s="76" t="s">
+      <c r="A106" s="102"/>
+      <c r="B106" s="101" t="s">
         <v>159</v>
       </c>
-      <c r="C106" s="75" t="s">
+      <c r="C106" s="100" t="s">
         <v>170</v>
       </c>
-      <c r="D106" s="74" t="s">
+      <c r="D106" s="99" t="s">
         <v>53</v>
       </c>
       <c r="E106" s="16" t="s">
@@ -43507,10 +43507,10 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A107" s="77"/>
-      <c r="B107" s="76"/>
-      <c r="C107" s="75"/>
-      <c r="D107" s="74"/>
+      <c r="A107" s="102"/>
+      <c r="B107" s="101"/>
+      <c r="C107" s="100"/>
+      <c r="D107" s="99"/>
       <c r="E107" s="16" t="s">
         <v>162</v>
       </c>
@@ -43519,10 +43519,10 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A108" s="77"/>
-      <c r="B108" s="76"/>
-      <c r="C108" s="75"/>
-      <c r="D108" s="74"/>
+      <c r="A108" s="102"/>
+      <c r="B108" s="101"/>
+      <c r="C108" s="100"/>
+      <c r="D108" s="99"/>
       <c r="E108" s="16" t="s">
         <v>330</v>
       </c>
@@ -43531,10 +43531,10 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A109" s="77"/>
-      <c r="B109" s="76"/>
-      <c r="C109" s="75"/>
-      <c r="D109" s="74"/>
+      <c r="A109" s="102"/>
+      <c r="B109" s="101"/>
+      <c r="C109" s="100"/>
+      <c r="D109" s="99"/>
       <c r="E109" s="16" t="s">
         <v>164</v>
       </c>
@@ -43543,10 +43543,10 @@
       </c>
     </row>
     <row r="110" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="77"/>
-      <c r="B110" s="76"/>
-      <c r="C110" s="75"/>
-      <c r="D110" s="74"/>
+      <c r="A110" s="102"/>
+      <c r="B110" s="101"/>
+      <c r="C110" s="100"/>
+      <c r="D110" s="99"/>
       <c r="E110" s="16" t="s">
         <v>166</v>
       </c>
@@ -43555,10 +43555,10 @@
       </c>
     </row>
     <row r="111" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="77"/>
-      <c r="B111" s="76"/>
-      <c r="C111" s="75"/>
-      <c r="D111" s="74"/>
+      <c r="A111" s="102"/>
+      <c r="B111" s="101"/>
+      <c r="C111" s="100"/>
+      <c r="D111" s="99"/>
       <c r="E111" s="16" t="s">
         <v>271</v>
       </c>
@@ -43567,10 +43567,10 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A112" s="77"/>
-      <c r="B112" s="76"/>
-      <c r="C112" s="75"/>
-      <c r="D112" s="74"/>
+      <c r="A112" s="102"/>
+      <c r="B112" s="101"/>
+      <c r="C112" s="100"/>
+      <c r="D112" s="99"/>
       <c r="E112" s="16" t="s">
         <v>168</v>
       </c>
@@ -43579,7 +43579,7 @@
       </c>
     </row>
     <row r="113" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A113" s="65" t="s">
+      <c r="A113" s="105" t="s">
         <v>31</v>
       </c>
       <c r="B113" s="27" t="s">
@@ -43595,14 +43595,14 @@
       <c r="F113" s="19"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A114" s="65"/>
-      <c r="B114" s="66" t="s">
+      <c r="A114" s="105"/>
+      <c r="B114" s="106" t="s">
         <v>171</v>
       </c>
-      <c r="C114" s="69" t="s">
+      <c r="C114" s="109" t="s">
         <v>1067</v>
       </c>
-      <c r="D114" s="87" t="s">
+      <c r="D114" s="94" t="s">
         <v>48</v>
       </c>
       <c r="E114" s="19" t="s">
@@ -43613,10 +43613,10 @@
       </c>
     </row>
     <row r="115" spans="1:7" ht="34" x14ac:dyDescent="0.2">
-      <c r="A115" s="65"/>
-      <c r="B115" s="67"/>
-      <c r="C115" s="70"/>
-      <c r="D115" s="88"/>
+      <c r="A115" s="105"/>
+      <c r="B115" s="107"/>
+      <c r="C115" s="110"/>
+      <c r="D115" s="95"/>
       <c r="E115" s="19" t="s">
         <v>173</v>
       </c>
@@ -43625,10 +43625,10 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A116" s="65"/>
-      <c r="B116" s="67"/>
-      <c r="C116" s="70"/>
-      <c r="D116" s="88"/>
+      <c r="A116" s="105"/>
+      <c r="B116" s="107"/>
+      <c r="C116" s="110"/>
+      <c r="D116" s="95"/>
       <c r="E116" s="19" t="s">
         <v>176</v>
       </c>
@@ -43637,10 +43637,10 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A117" s="65"/>
-      <c r="B117" s="67"/>
-      <c r="C117" s="70"/>
-      <c r="D117" s="88"/>
+      <c r="A117" s="105"/>
+      <c r="B117" s="107"/>
+      <c r="C117" s="110"/>
+      <c r="D117" s="95"/>
       <c r="E117" s="19" t="s">
         <v>178</v>
       </c>
@@ -43649,10 +43649,10 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A118" s="65"/>
-      <c r="B118" s="67"/>
-      <c r="C118" s="70"/>
-      <c r="D118" s="88"/>
+      <c r="A118" s="105"/>
+      <c r="B118" s="107"/>
+      <c r="C118" s="110"/>
+      <c r="D118" s="95"/>
       <c r="E118" s="19" t="s">
         <v>175</v>
       </c>
@@ -43661,10 +43661,10 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A119" s="65"/>
-      <c r="B119" s="67"/>
-      <c r="C119" s="70"/>
-      <c r="D119" s="88"/>
+      <c r="A119" s="105"/>
+      <c r="B119" s="107"/>
+      <c r="C119" s="110"/>
+      <c r="D119" s="95"/>
       <c r="E119" s="19" t="s">
         <v>179</v>
       </c>
@@ -43673,10 +43673,10 @@
       </c>
     </row>
     <row r="120" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A120" s="65"/>
-      <c r="B120" s="67"/>
-      <c r="C120" s="70"/>
-      <c r="D120" s="88"/>
+      <c r="A120" s="105"/>
+      <c r="B120" s="107"/>
+      <c r="C120" s="110"/>
+      <c r="D120" s="95"/>
       <c r="E120" s="19" t="s">
         <v>181</v>
       </c>
@@ -43685,10 +43685,10 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="17" x14ac:dyDescent="0.2">
-      <c r="A121" s="65"/>
-      <c r="B121" s="68"/>
-      <c r="C121" s="71"/>
-      <c r="D121" s="89"/>
+      <c r="A121" s="105"/>
+      <c r="B121" s="108"/>
+      <c r="C121" s="111"/>
+      <c r="D121" s="96"/>
       <c r="E121" s="19" t="s">
         <v>336</v>
       </c>
@@ -43697,7 +43697,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="85" x14ac:dyDescent="0.2">
-      <c r="A122" s="65"/>
+      <c r="A122" s="105"/>
       <c r="B122" s="27" t="s">
         <v>31</v>
       </c>
@@ -43711,14 +43711,14 @@
       <c r="F122" s="19"/>
     </row>
     <row r="123" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="65"/>
-      <c r="B123" s="86" t="s">
+      <c r="A123" s="105"/>
+      <c r="B123" s="67" t="s">
         <v>183</v>
       </c>
-      <c r="C123" s="58" t="s">
+      <c r="C123" s="76" t="s">
         <v>246</v>
       </c>
-      <c r="D123" s="85" t="s">
+      <c r="D123" s="75" t="s">
         <v>48</v>
       </c>
       <c r="E123" s="19" t="s">
@@ -43730,10 +43730,10 @@
       <c r="G123" s="21"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A124" s="65"/>
-      <c r="B124" s="86"/>
-      <c r="C124" s="58"/>
-      <c r="D124" s="85"/>
+      <c r="A124" s="105"/>
+      <c r="B124" s="67"/>
+      <c r="C124" s="76"/>
+      <c r="D124" s="75"/>
       <c r="E124" s="19" t="s">
         <v>204</v>
       </c>
@@ -43743,10 +43743,10 @@
       <c r="G124" s="21"/>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A125" s="65"/>
-      <c r="B125" s="86"/>
-      <c r="C125" s="58"/>
-      <c r="D125" s="85"/>
+      <c r="A125" s="105"/>
+      <c r="B125" s="67"/>
+      <c r="C125" s="76"/>
+      <c r="D125" s="75"/>
       <c r="E125" s="19" t="s">
         <v>205</v>
       </c>
@@ -43756,10 +43756,10 @@
       <c r="G125" s="21"/>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A126" s="65"/>
-      <c r="B126" s="86"/>
-      <c r="C126" s="58"/>
-      <c r="D126" s="85"/>
+      <c r="A126" s="105"/>
+      <c r="B126" s="67"/>
+      <c r="C126" s="76"/>
+      <c r="D126" s="75"/>
       <c r="E126" s="19" t="s">
         <v>381</v>
       </c>
@@ -43769,10 +43769,10 @@
       <c r="G126" s="21"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A127" s="65"/>
-      <c r="B127" s="86"/>
-      <c r="C127" s="58"/>
-      <c r="D127" s="85"/>
+      <c r="A127" s="105"/>
+      <c r="B127" s="67"/>
+      <c r="C127" s="76"/>
+      <c r="D127" s="75"/>
       <c r="E127" s="19" t="s">
         <v>206</v>
       </c>
@@ -43782,10 +43782,10 @@
       <c r="G127" s="21"/>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A128" s="65"/>
-      <c r="B128" s="86"/>
-      <c r="C128" s="58"/>
-      <c r="D128" s="85"/>
+      <c r="A128" s="105"/>
+      <c r="B128" s="67"/>
+      <c r="C128" s="76"/>
+      <c r="D128" s="75"/>
       <c r="E128" s="19" t="s">
         <v>207</v>
       </c>
@@ -43795,10 +43795,10 @@
       <c r="G128" s="21"/>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A129" s="65"/>
-      <c r="B129" s="86"/>
-      <c r="C129" s="58"/>
-      <c r="D129" s="85"/>
+      <c r="A129" s="105"/>
+      <c r="B129" s="67"/>
+      <c r="C129" s="76"/>
+      <c r="D129" s="75"/>
       <c r="E129" s="19" t="s">
         <v>208</v>
       </c>
@@ -43808,10 +43808,10 @@
       <c r="G129" s="21"/>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A130" s="65"/>
-      <c r="B130" s="86"/>
-      <c r="C130" s="58"/>
-      <c r="D130" s="85"/>
+      <c r="A130" s="105"/>
+      <c r="B130" s="67"/>
+      <c r="C130" s="76"/>
+      <c r="D130" s="75"/>
       <c r="E130" s="19" t="s">
         <v>354</v>
       </c>
@@ -43821,10 +43821,10 @@
       <c r="G130" s="21"/>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A131" s="65"/>
-      <c r="B131" s="86"/>
-      <c r="C131" s="58"/>
-      <c r="D131" s="85"/>
+      <c r="A131" s="105"/>
+      <c r="B131" s="67"/>
+      <c r="C131" s="76"/>
+      <c r="D131" s="75"/>
       <c r="E131" s="19" t="s">
         <v>209</v>
       </c>
@@ -43834,10 +43834,10 @@
       <c r="G131" s="21"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A132" s="65"/>
-      <c r="B132" s="86"/>
-      <c r="C132" s="58"/>
-      <c r="D132" s="85"/>
+      <c r="A132" s="105"/>
+      <c r="B132" s="67"/>
+      <c r="C132" s="76"/>
+      <c r="D132" s="75"/>
       <c r="E132" s="19" t="s">
         <v>352</v>
       </c>
@@ -43847,10 +43847,10 @@
       <c r="G132" s="21"/>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A133" s="65"/>
-      <c r="B133" s="86"/>
-      <c r="C133" s="58"/>
-      <c r="D133" s="85"/>
+      <c r="A133" s="105"/>
+      <c r="B133" s="67"/>
+      <c r="C133" s="76"/>
+      <c r="D133" s="75"/>
       <c r="E133" s="19" t="s">
         <v>210</v>
       </c>
@@ -43860,10 +43860,10 @@
       <c r="G133" s="21"/>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A134" s="65"/>
-      <c r="B134" s="86"/>
-      <c r="C134" s="58"/>
-      <c r="D134" s="85"/>
+      <c r="A134" s="105"/>
+      <c r="B134" s="67"/>
+      <c r="C134" s="76"/>
+      <c r="D134" s="75"/>
       <c r="E134" s="19" t="s">
         <v>211</v>
       </c>
@@ -43873,10 +43873,10 @@
       <c r="G134" s="21"/>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A135" s="65"/>
-      <c r="B135" s="86"/>
-      <c r="C135" s="58"/>
-      <c r="D135" s="85"/>
+      <c r="A135" s="105"/>
+      <c r="B135" s="67"/>
+      <c r="C135" s="76"/>
+      <c r="D135" s="75"/>
       <c r="E135" s="19" t="s">
         <v>212</v>
       </c>
@@ -43886,10 +43886,10 @@
       <c r="G135" s="21"/>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A136" s="65"/>
-      <c r="B136" s="86"/>
-      <c r="C136" s="58"/>
-      <c r="D136" s="85"/>
+      <c r="A136" s="105"/>
+      <c r="B136" s="67"/>
+      <c r="C136" s="76"/>
+      <c r="D136" s="75"/>
       <c r="E136" s="19" t="s">
         <v>335</v>
       </c>
@@ -43899,10 +43899,10 @@
       <c r="G136" s="21"/>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A137" s="65"/>
-      <c r="B137" s="86"/>
-      <c r="C137" s="58"/>
-      <c r="D137" s="85"/>
+      <c r="A137" s="105"/>
+      <c r="B137" s="67"/>
+      <c r="C137" s="76"/>
+      <c r="D137" s="75"/>
       <c r="E137" s="19" t="s">
         <v>213</v>
       </c>
@@ -43912,10 +43912,10 @@
       <c r="G137" s="21"/>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A138" s="65"/>
-      <c r="B138" s="86"/>
-      <c r="C138" s="58"/>
-      <c r="D138" s="85"/>
+      <c r="A138" s="105"/>
+      <c r="B138" s="67"/>
+      <c r="C138" s="76"/>
+      <c r="D138" s="75"/>
       <c r="E138" s="19" t="s">
         <v>199</v>
       </c>
@@ -43925,10 +43925,10 @@
       <c r="G138" s="21"/>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A139" s="65"/>
-      <c r="B139" s="86"/>
-      <c r="C139" s="58"/>
-      <c r="D139" s="85"/>
+      <c r="A139" s="105"/>
+      <c r="B139" s="67"/>
+      <c r="C139" s="76"/>
+      <c r="D139" s="75"/>
       <c r="E139" s="19" t="s">
         <v>214</v>
       </c>
@@ -43938,10 +43938,10 @@
       <c r="G139" s="21"/>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A140" s="65"/>
-      <c r="B140" s="86"/>
-      <c r="C140" s="58"/>
-      <c r="D140" s="85"/>
+      <c r="A140" s="105"/>
+      <c r="B140" s="67"/>
+      <c r="C140" s="76"/>
+      <c r="D140" s="75"/>
       <c r="E140" s="19" t="s">
         <v>215</v>
       </c>
@@ -43951,10 +43951,10 @@
       <c r="G140" s="21"/>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A141" s="65"/>
-      <c r="B141" s="86"/>
-      <c r="C141" s="58"/>
-      <c r="D141" s="85"/>
+      <c r="A141" s="105"/>
+      <c r="B141" s="67"/>
+      <c r="C141" s="76"/>
+      <c r="D141" s="75"/>
       <c r="E141" s="19" t="s">
         <v>216</v>
       </c>
@@ -43964,10 +43964,10 @@
       <c r="G141" s="21"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A142" s="65"/>
-      <c r="B142" s="86"/>
-      <c r="C142" s="58"/>
-      <c r="D142" s="85"/>
+      <c r="A142" s="105"/>
+      <c r="B142" s="67"/>
+      <c r="C142" s="76"/>
+      <c r="D142" s="75"/>
       <c r="E142" s="19" t="s">
         <v>217</v>
       </c>
@@ -43977,10 +43977,10 @@
       <c r="G142" s="21"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A143" s="65"/>
-      <c r="B143" s="86"/>
-      <c r="C143" s="58"/>
-      <c r="D143" s="85"/>
+      <c r="A143" s="105"/>
+      <c r="B143" s="67"/>
+      <c r="C143" s="76"/>
+      <c r="D143" s="75"/>
       <c r="E143" s="19" t="s">
         <v>218</v>
       </c>
@@ -43990,10 +43990,10 @@
       <c r="G143" s="21"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A144" s="65"/>
-      <c r="B144" s="86"/>
-      <c r="C144" s="58"/>
-      <c r="D144" s="85"/>
+      <c r="A144" s="105"/>
+      <c r="B144" s="67"/>
+      <c r="C144" s="76"/>
+      <c r="D144" s="75"/>
       <c r="E144" s="19" t="s">
         <v>201</v>
       </c>
@@ -44003,14 +44003,14 @@
       <c r="G144" s="21"/>
     </row>
     <row r="145" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A145" s="65"/>
-      <c r="B145" s="86" t="s">
+      <c r="A145" s="105"/>
+      <c r="B145" s="67" t="s">
         <v>219</v>
       </c>
-      <c r="C145" s="58" t="s">
+      <c r="C145" s="76" t="s">
         <v>220</v>
       </c>
-      <c r="D145" s="85" t="s">
+      <c r="D145" s="75" t="s">
         <v>48</v>
       </c>
       <c r="E145" s="19" t="s">
@@ -44021,10 +44021,10 @@
       </c>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A146" s="65"/>
-      <c r="B146" s="86"/>
-      <c r="C146" s="58"/>
-      <c r="D146" s="85"/>
+      <c r="A146" s="105"/>
+      <c r="B146" s="67"/>
+      <c r="C146" s="76"/>
+      <c r="D146" s="75"/>
       <c r="E146" s="19" t="s">
         <v>223</v>
       </c>
@@ -44033,10 +44033,10 @@
       </c>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A147" s="65"/>
-      <c r="B147" s="86"/>
-      <c r="C147" s="58"/>
-      <c r="D147" s="85"/>
+      <c r="A147" s="105"/>
+      <c r="B147" s="67"/>
+      <c r="C147" s="76"/>
+      <c r="D147" s="75"/>
       <c r="E147" s="19" t="s">
         <v>226</v>
       </c>
@@ -44045,10 +44045,10 @@
       </c>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A148" s="65"/>
-      <c r="B148" s="86"/>
-      <c r="C148" s="58"/>
-      <c r="D148" s="85"/>
+      <c r="A148" s="105"/>
+      <c r="B148" s="67"/>
+      <c r="C148" s="76"/>
+      <c r="D148" s="75"/>
       <c r="E148" s="19" t="s">
         <v>222</v>
       </c>
@@ -44057,10 +44057,10 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A149" s="65"/>
-      <c r="B149" s="86"/>
-      <c r="C149" s="58"/>
-      <c r="D149" s="85"/>
+      <c r="A149" s="105"/>
+      <c r="B149" s="67"/>
+      <c r="C149" s="76"/>
+      <c r="D149" s="75"/>
       <c r="E149" s="19" t="s">
         <v>196</v>
       </c>
@@ -44069,14 +44069,14 @@
       </c>
     </row>
     <row r="150" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A150" s="65"/>
-      <c r="B150" s="86" t="s">
+      <c r="A150" s="105"/>
+      <c r="B150" s="67" t="s">
         <v>181</v>
       </c>
-      <c r="C150" s="111" t="s">
+      <c r="C150" s="74" t="s">
         <v>228</v>
       </c>
-      <c r="D150" s="85" t="s">
+      <c r="D150" s="75" t="s">
         <v>48</v>
       </c>
       <c r="E150" s="19" t="s">
@@ -44087,10 +44087,10 @@
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A151" s="65"/>
-      <c r="B151" s="86"/>
-      <c r="C151" s="111"/>
-      <c r="D151" s="85"/>
+      <c r="A151" s="105"/>
+      <c r="B151" s="67"/>
+      <c r="C151" s="74"/>
+      <c r="D151" s="75"/>
       <c r="E151" s="19" t="s">
         <v>230</v>
       </c>
@@ -44099,10 +44099,10 @@
       </c>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A152" s="65"/>
-      <c r="B152" s="86"/>
-      <c r="C152" s="111"/>
-      <c r="D152" s="85"/>
+      <c r="A152" s="105"/>
+      <c r="B152" s="67"/>
+      <c r="C152" s="74"/>
+      <c r="D152" s="75"/>
       <c r="E152" s="19" t="s">
         <v>231</v>
       </c>
@@ -44111,14 +44111,14 @@
       </c>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A153" s="65"/>
-      <c r="B153" s="86" t="s">
+      <c r="A153" s="105"/>
+      <c r="B153" s="67" t="s">
         <v>237</v>
       </c>
-      <c r="C153" s="58" t="s">
+      <c r="C153" s="76" t="s">
         <v>238</v>
       </c>
-      <c r="D153" s="85" t="s">
+      <c r="D153" s="75" t="s">
         <v>48</v>
       </c>
       <c r="E153" s="19" t="s">
@@ -44129,10 +44129,10 @@
       </c>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A154" s="65"/>
-      <c r="B154" s="86"/>
-      <c r="C154" s="58"/>
-      <c r="D154" s="85"/>
+      <c r="A154" s="105"/>
+      <c r="B154" s="67"/>
+      <c r="C154" s="76"/>
+      <c r="D154" s="75"/>
       <c r="E154" s="19" t="s">
         <v>243</v>
       </c>
@@ -44141,10 +44141,10 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A155" s="65"/>
-      <c r="B155" s="86"/>
-      <c r="C155" s="58"/>
-      <c r="D155" s="85"/>
+      <c r="A155" s="105"/>
+      <c r="B155" s="67"/>
+      <c r="C155" s="76"/>
+      <c r="D155" s="75"/>
       <c r="E155" s="19" t="s">
         <v>231</v>
       </c>
@@ -44153,10 +44153,10 @@
       </c>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A156" s="65"/>
-      <c r="B156" s="86"/>
-      <c r="C156" s="58"/>
-      <c r="D156" s="85"/>
+      <c r="A156" s="105"/>
+      <c r="B156" s="67"/>
+      <c r="C156" s="76"/>
+      <c r="D156" s="75"/>
       <c r="E156" s="19" t="s">
         <v>244</v>
       </c>
@@ -44165,16 +44165,16 @@
       </c>
     </row>
     <row r="157" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="55" t="s">
+      <c r="A157" s="103" t="s">
         <v>247</v>
       </c>
-      <c r="B157" s="62" t="s">
+      <c r="B157" s="55" t="s">
         <v>305</v>
       </c>
-      <c r="C157" s="59" t="s">
+      <c r="C157" s="58" t="s">
         <v>1071</v>
       </c>
-      <c r="D157" s="59" t="s">
+      <c r="D157" s="58" t="s">
         <v>48</v>
       </c>
       <c r="E157" s="22" t="s">
@@ -44185,10 +44185,10 @@
       </c>
     </row>
     <row r="158" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A158" s="55"/>
-      <c r="B158" s="63"/>
-      <c r="C158" s="60"/>
-      <c r="D158" s="60"/>
+      <c r="A158" s="103"/>
+      <c r="B158" s="56"/>
+      <c r="C158" s="73"/>
+      <c r="D158" s="73"/>
       <c r="E158" s="22" t="s">
         <v>173</v>
       </c>
@@ -44197,10 +44197,10 @@
       </c>
     </row>
     <row r="159" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A159" s="55"/>
-      <c r="B159" s="63"/>
-      <c r="C159" s="60"/>
-      <c r="D159" s="60"/>
+      <c r="A159" s="103"/>
+      <c r="B159" s="56"/>
+      <c r="C159" s="73"/>
+      <c r="D159" s="73"/>
       <c r="E159" s="22" t="s">
         <v>251</v>
       </c>
@@ -44209,10 +44209,10 @@
       </c>
     </row>
     <row r="160" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A160" s="55"/>
-      <c r="B160" s="63"/>
-      <c r="C160" s="60"/>
-      <c r="D160" s="60"/>
+      <c r="A160" s="103"/>
+      <c r="B160" s="56"/>
+      <c r="C160" s="73"/>
+      <c r="D160" s="73"/>
       <c r="E160" s="22" t="s">
         <v>253</v>
       </c>
@@ -44221,10 +44221,10 @@
       </c>
     </row>
     <row r="161" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A161" s="55"/>
-      <c r="B161" s="63"/>
-      <c r="C161" s="60"/>
-      <c r="D161" s="60"/>
+      <c r="A161" s="103"/>
+      <c r="B161" s="56"/>
+      <c r="C161" s="73"/>
+      <c r="D161" s="73"/>
       <c r="E161" s="22" t="s">
         <v>255</v>
       </c>
@@ -44233,10 +44233,10 @@
       </c>
     </row>
     <row r="162" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A162" s="55"/>
-      <c r="B162" s="63"/>
-      <c r="C162" s="60"/>
-      <c r="D162" s="60"/>
+      <c r="A162" s="103"/>
+      <c r="B162" s="56"/>
+      <c r="C162" s="73"/>
+      <c r="D162" s="73"/>
       <c r="E162" s="22" t="s">
         <v>257</v>
       </c>
@@ -44245,10 +44245,10 @@
       </c>
     </row>
     <row r="163" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A163" s="55"/>
-      <c r="B163" s="63"/>
-      <c r="C163" s="60"/>
-      <c r="D163" s="60"/>
+      <c r="A163" s="103"/>
+      <c r="B163" s="56"/>
+      <c r="C163" s="73"/>
+      <c r="D163" s="73"/>
       <c r="E163" s="22" t="s">
         <v>333</v>
       </c>
@@ -44257,10 +44257,10 @@
       </c>
     </row>
     <row r="164" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A164" s="55"/>
-      <c r="B164" s="64"/>
-      <c r="C164" s="61"/>
-      <c r="D164" s="61"/>
+      <c r="A164" s="103"/>
+      <c r="B164" s="57"/>
+      <c r="C164" s="59"/>
+      <c r="D164" s="59"/>
       <c r="E164" s="22" t="s">
         <v>323</v>
       </c>
@@ -44269,14 +44269,14 @@
       </c>
     </row>
     <row r="165" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A165" s="55"/>
-      <c r="B165" s="62" t="s">
+      <c r="A165" s="103"/>
+      <c r="B165" s="55" t="s">
         <v>304</v>
       </c>
-      <c r="C165" s="59" t="s">
+      <c r="C165" s="58" t="s">
         <v>1076</v>
       </c>
-      <c r="D165" s="59" t="s">
+      <c r="D165" s="58" t="s">
         <v>48</v>
       </c>
       <c r="E165" s="22" t="s">
@@ -44285,24 +44285,24 @@
       <c r="F165" s="22"/>
     </row>
     <row r="166" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A166" s="55"/>
-      <c r="B166" s="64"/>
-      <c r="C166" s="61"/>
-      <c r="D166" s="61"/>
+      <c r="A166" s="103"/>
+      <c r="B166" s="57"/>
+      <c r="C166" s="59"/>
+      <c r="D166" s="59"/>
       <c r="E166" s="22" t="s">
         <v>261</v>
       </c>
       <c r="F166" s="22"/>
     </row>
     <row r="167" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A167" s="55"/>
-      <c r="B167" s="56" t="s">
+      <c r="A167" s="103"/>
+      <c r="B167" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="C167" s="57" t="s">
+      <c r="C167" s="77" t="s">
         <v>1075</v>
       </c>
-      <c r="D167" s="57" t="s">
+      <c r="D167" s="77" t="s">
         <v>53</v>
       </c>
       <c r="E167" s="22" t="s">
@@ -44313,10 +44313,10 @@
       </c>
     </row>
     <row r="168" spans="1:6" ht="34" x14ac:dyDescent="0.2">
-      <c r="A168" s="55"/>
-      <c r="B168" s="56"/>
-      <c r="C168" s="57"/>
-      <c r="D168" s="57"/>
+      <c r="A168" s="103"/>
+      <c r="B168" s="104"/>
+      <c r="C168" s="77"/>
+      <c r="D168" s="77"/>
       <c r="E168" s="22" t="s">
         <v>179</v>
       </c>
@@ -44325,10 +44325,10 @@
       </c>
     </row>
     <row r="169" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A169" s="55"/>
-      <c r="B169" s="56"/>
-      <c r="C169" s="57"/>
-      <c r="D169" s="57"/>
+      <c r="A169" s="103"/>
+      <c r="B169" s="104"/>
+      <c r="C169" s="77"/>
+      <c r="D169" s="77"/>
       <c r="E169" s="22" t="s">
         <v>259</v>
       </c>
@@ -44337,14 +44337,14 @@
       </c>
     </row>
     <row r="170" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A170" s="55"/>
-      <c r="B170" s="62" t="s">
+      <c r="A170" s="103"/>
+      <c r="B170" s="55" t="s">
         <v>262</v>
       </c>
-      <c r="C170" s="59" t="s">
+      <c r="C170" s="58" t="s">
         <v>1074</v>
       </c>
-      <c r="D170" s="59" t="s">
+      <c r="D170" s="58" t="s">
         <v>48</v>
       </c>
       <c r="E170" s="22" t="s">
@@ -44355,10 +44355,10 @@
       </c>
     </row>
     <row r="171" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="55"/>
-      <c r="B171" s="63"/>
-      <c r="C171" s="60"/>
-      <c r="D171" s="60"/>
+      <c r="A171" s="103"/>
+      <c r="B171" s="56"/>
+      <c r="C171" s="73"/>
+      <c r="D171" s="73"/>
       <c r="E171" s="22" t="s">
         <v>298</v>
       </c>
@@ -44367,10 +44367,10 @@
       </c>
     </row>
     <row r="172" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="55"/>
-      <c r="B172" s="63"/>
-      <c r="C172" s="60"/>
-      <c r="D172" s="60"/>
+      <c r="A172" s="103"/>
+      <c r="B172" s="56"/>
+      <c r="C172" s="73"/>
+      <c r="D172" s="73"/>
       <c r="E172" s="22" t="s">
         <v>443</v>
       </c>
@@ -44379,10 +44379,10 @@
       </c>
     </row>
     <row r="173" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A173" s="55"/>
-      <c r="B173" s="63"/>
-      <c r="C173" s="60"/>
-      <c r="D173" s="60"/>
+      <c r="A173" s="103"/>
+      <c r="B173" s="56"/>
+      <c r="C173" s="73"/>
+      <c r="D173" s="73"/>
       <c r="E173" s="22" t="s">
         <v>299</v>
       </c>
@@ -44391,10 +44391,10 @@
       </c>
     </row>
     <row r="174" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="55"/>
-      <c r="B174" s="63"/>
-      <c r="C174" s="60"/>
-      <c r="D174" s="60"/>
+      <c r="A174" s="103"/>
+      <c r="B174" s="56"/>
+      <c r="C174" s="73"/>
+      <c r="D174" s="73"/>
       <c r="E174" s="22" t="s">
         <v>297</v>
       </c>
@@ -44403,10 +44403,10 @@
       </c>
     </row>
     <row r="175" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="55"/>
-      <c r="B175" s="63"/>
-      <c r="C175" s="60"/>
-      <c r="D175" s="60"/>
+      <c r="A175" s="103"/>
+      <c r="B175" s="56"/>
+      <c r="C175" s="73"/>
+      <c r="D175" s="73"/>
       <c r="E175" s="22" t="s">
         <v>300</v>
       </c>
@@ -44415,10 +44415,10 @@
       </c>
     </row>
     <row r="176" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="55"/>
-      <c r="B176" s="63"/>
-      <c r="C176" s="60"/>
-      <c r="D176" s="60"/>
+      <c r="A176" s="103"/>
+      <c r="B176" s="56"/>
+      <c r="C176" s="73"/>
+      <c r="D176" s="73"/>
       <c r="E176" s="22" t="s">
         <v>302</v>
       </c>
@@ -44427,10 +44427,10 @@
       </c>
     </row>
     <row r="177" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="55"/>
-      <c r="B177" s="64"/>
-      <c r="C177" s="61"/>
-      <c r="D177" s="61"/>
+      <c r="A177" s="103"/>
+      <c r="B177" s="57"/>
+      <c r="C177" s="59"/>
+      <c r="D177" s="59"/>
       <c r="E177" s="22" t="s">
         <v>57</v>
       </c>
@@ -44439,14 +44439,14 @@
       </c>
     </row>
     <row r="178" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="55"/>
-      <c r="B178" s="56" t="s">
+      <c r="A178" s="103"/>
+      <c r="B178" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="C178" s="57" t="s">
+      <c r="C178" s="77" t="s">
         <v>1077</v>
       </c>
-      <c r="D178" s="57" t="s">
+      <c r="D178" s="77" t="s">
         <v>53</v>
       </c>
       <c r="E178" s="22" t="s">
@@ -44457,10 +44457,10 @@
       </c>
     </row>
     <row r="179" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A179" s="55"/>
-      <c r="B179" s="56"/>
-      <c r="C179" s="57"/>
-      <c r="D179" s="57"/>
+      <c r="A179" s="103"/>
+      <c r="B179" s="104"/>
+      <c r="C179" s="77"/>
+      <c r="D179" s="77"/>
       <c r="E179" s="22" t="s">
         <v>264</v>
       </c>
@@ -44469,10 +44469,10 @@
       </c>
     </row>
     <row r="180" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A180" s="55"/>
-      <c r="B180" s="56"/>
-      <c r="C180" s="57"/>
-      <c r="D180" s="57"/>
+      <c r="A180" s="103"/>
+      <c r="B180" s="104"/>
+      <c r="C180" s="77"/>
+      <c r="D180" s="77"/>
       <c r="E180" s="22" t="s">
         <v>267</v>
       </c>
@@ -44481,10 +44481,10 @@
       </c>
     </row>
     <row r="181" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A181" s="55"/>
-      <c r="B181" s="56"/>
-      <c r="C181" s="57"/>
-      <c r="D181" s="57"/>
+      <c r="A181" s="103"/>
+      <c r="B181" s="104"/>
+      <c r="C181" s="77"/>
+      <c r="D181" s="77"/>
       <c r="E181" s="22" t="s">
         <v>269</v>
       </c>
@@ -44493,10 +44493,10 @@
       </c>
     </row>
     <row r="182" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A182" s="55"/>
-      <c r="B182" s="56"/>
-      <c r="C182" s="57"/>
-      <c r="D182" s="57"/>
+      <c r="A182" s="103"/>
+      <c r="B182" s="104"/>
+      <c r="C182" s="77"/>
+      <c r="D182" s="77"/>
       <c r="E182" s="22" t="s">
         <v>271</v>
       </c>
@@ -44505,10 +44505,10 @@
       </c>
     </row>
     <row r="183" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A183" s="55"/>
-      <c r="B183" s="56"/>
-      <c r="C183" s="57"/>
-      <c r="D183" s="57"/>
+      <c r="A183" s="103"/>
+      <c r="B183" s="104"/>
+      <c r="C183" s="77"/>
+      <c r="D183" s="77"/>
       <c r="E183" s="22" t="s">
         <v>273</v>
       </c>
@@ -44517,10 +44517,10 @@
       </c>
     </row>
     <row r="184" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A184" s="55"/>
-      <c r="B184" s="56"/>
-      <c r="C184" s="57"/>
-      <c r="D184" s="57"/>
+      <c r="A184" s="103"/>
+      <c r="B184" s="104"/>
+      <c r="C184" s="77"/>
+      <c r="D184" s="77"/>
       <c r="E184" s="22" t="s">
         <v>276</v>
       </c>
@@ -44529,10 +44529,10 @@
       </c>
     </row>
     <row r="185" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A185" s="55"/>
-      <c r="B185" s="56"/>
-      <c r="C185" s="57"/>
-      <c r="D185" s="57"/>
+      <c r="A185" s="103"/>
+      <c r="B185" s="104"/>
+      <c r="C185" s="77"/>
+      <c r="D185" s="77"/>
       <c r="E185" s="22" t="s">
         <v>282</v>
       </c>
@@ -44541,10 +44541,10 @@
       </c>
     </row>
     <row r="186" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A186" s="55"/>
-      <c r="B186" s="56"/>
-      <c r="C186" s="57"/>
-      <c r="D186" s="57"/>
+      <c r="A186" s="103"/>
+      <c r="B186" s="104"/>
+      <c r="C186" s="77"/>
+      <c r="D186" s="77"/>
       <c r="E186" s="22" t="s">
         <v>57</v>
       </c>
@@ -44553,14 +44553,14 @@
       </c>
     </row>
     <row r="187" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A187" s="55"/>
-      <c r="B187" s="62" t="s">
+      <c r="A187" s="103"/>
+      <c r="B187" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C187" s="59" t="s">
+      <c r="C187" s="58" t="s">
         <v>1073</v>
       </c>
-      <c r="D187" s="59" t="s">
+      <c r="D187" s="58" t="s">
         <v>48</v>
       </c>
       <c r="E187" s="22" t="s">
@@ -44571,10 +44571,10 @@
       </c>
     </row>
     <row r="188" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A188" s="55"/>
-      <c r="B188" s="63"/>
-      <c r="C188" s="60"/>
-      <c r="D188" s="60"/>
+      <c r="A188" s="103"/>
+      <c r="B188" s="56"/>
+      <c r="C188" s="73"/>
+      <c r="D188" s="73"/>
       <c r="E188" s="22" t="s">
         <v>277</v>
       </c>
@@ -44583,10 +44583,10 @@
       </c>
     </row>
     <row r="189" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A189" s="55"/>
-      <c r="B189" s="63"/>
-      <c r="C189" s="60"/>
-      <c r="D189" s="60"/>
+      <c r="A189" s="103"/>
+      <c r="B189" s="56"/>
+      <c r="C189" s="73"/>
+      <c r="D189" s="73"/>
       <c r="E189" s="22" t="s">
         <v>405</v>
       </c>
@@ -44595,10 +44595,10 @@
       </c>
     </row>
     <row r="190" spans="1:6" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A190" s="55"/>
-      <c r="B190" s="63"/>
-      <c r="C190" s="60"/>
-      <c r="D190" s="60"/>
+      <c r="A190" s="103"/>
+      <c r="B190" s="56"/>
+      <c r="C190" s="73"/>
+      <c r="D190" s="73"/>
       <c r="E190" s="22" t="s">
         <v>278</v>
       </c>
@@ -44607,10 +44607,10 @@
       </c>
     </row>
     <row r="191" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A191" s="55"/>
-      <c r="B191" s="63"/>
-      <c r="C191" s="60"/>
-      <c r="D191" s="60"/>
+      <c r="A191" s="103"/>
+      <c r="B191" s="56"/>
+      <c r="C191" s="73"/>
+      <c r="D191" s="73"/>
       <c r="E191" s="22" t="s">
         <v>281</v>
       </c>
@@ -44619,10 +44619,10 @@
       </c>
     </row>
     <row r="192" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A192" s="55"/>
-      <c r="B192" s="63"/>
-      <c r="C192" s="60"/>
-      <c r="D192" s="60"/>
+      <c r="A192" s="103"/>
+      <c r="B192" s="56"/>
+      <c r="C192" s="73"/>
+      <c r="D192" s="73"/>
       <c r="E192" s="22" t="s">
         <v>57</v>
       </c>
@@ -44631,10 +44631,10 @@
       </c>
     </row>
     <row r="193" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A193" s="55"/>
-      <c r="B193" s="64"/>
-      <c r="C193" s="61"/>
-      <c r="D193" s="61"/>
+      <c r="A193" s="103"/>
+      <c r="B193" s="57"/>
+      <c r="C193" s="59"/>
+      <c r="D193" s="59"/>
       <c r="E193" s="22" t="s">
         <v>81</v>
       </c>
@@ -44643,14 +44643,14 @@
       </c>
     </row>
     <row r="194" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A194" s="55"/>
-      <c r="B194" s="56" t="s">
+      <c r="A194" s="103"/>
+      <c r="B194" s="104" t="s">
         <v>35</v>
       </c>
-      <c r="C194" s="57" t="s">
+      <c r="C194" s="77" t="s">
         <v>1078</v>
       </c>
-      <c r="D194" s="57" t="s">
+      <c r="D194" s="77" t="s">
         <v>53</v>
       </c>
       <c r="E194" s="22" t="s">
@@ -44661,10 +44661,10 @@
       </c>
     </row>
     <row r="195" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A195" s="55"/>
-      <c r="B195" s="56"/>
-      <c r="C195" s="57"/>
-      <c r="D195" s="57"/>
+      <c r="A195" s="103"/>
+      <c r="B195" s="104"/>
+      <c r="C195" s="77"/>
+      <c r="D195" s="77"/>
       <c r="E195" s="22" t="s">
         <v>358</v>
       </c>
@@ -44673,10 +44673,10 @@
       </c>
     </row>
     <row r="196" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A196" s="55"/>
-      <c r="B196" s="56"/>
-      <c r="C196" s="57"/>
-      <c r="D196" s="57"/>
+      <c r="A196" s="103"/>
+      <c r="B196" s="104"/>
+      <c r="C196" s="77"/>
+      <c r="D196" s="77"/>
       <c r="E196" s="22" t="s">
         <v>334</v>
       </c>
@@ -44685,10 +44685,10 @@
       </c>
     </row>
     <row r="197" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A197" s="55"/>
-      <c r="B197" s="56"/>
-      <c r="C197" s="57"/>
-      <c r="D197" s="57"/>
+      <c r="A197" s="103"/>
+      <c r="B197" s="104"/>
+      <c r="C197" s="77"/>
+      <c r="D197" s="77"/>
       <c r="E197" s="22" t="s">
         <v>285</v>
       </c>
@@ -44697,10 +44697,10 @@
       </c>
     </row>
     <row r="198" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A198" s="55"/>
-      <c r="B198" s="56"/>
-      <c r="C198" s="57"/>
-      <c r="D198" s="57"/>
+      <c r="A198" s="103"/>
+      <c r="B198" s="104"/>
+      <c r="C198" s="77"/>
+      <c r="D198" s="77"/>
       <c r="E198" s="22" t="s">
         <v>286</v>
       </c>
@@ -44709,10 +44709,10 @@
       </c>
     </row>
     <row r="199" spans="1:6" ht="17" x14ac:dyDescent="0.2">
-      <c r="A199" s="55"/>
-      <c r="B199" s="56"/>
-      <c r="C199" s="57"/>
-      <c r="D199" s="57"/>
+      <c r="A199" s="103"/>
+      <c r="B199" s="104"/>
+      <c r="C199" s="77"/>
+      <c r="D199" s="77"/>
       <c r="E199" s="22" t="s">
         <v>96</v>
       </c>
@@ -44727,33 +44727,48 @@
     <row r="206" spans="1:6" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="85">
-    <mergeCell ref="B170:B177"/>
-    <mergeCell ref="D165:D166"/>
-    <mergeCell ref="C165:C166"/>
-    <mergeCell ref="B165:B166"/>
-    <mergeCell ref="B28:B33"/>
-    <mergeCell ref="C95:C98"/>
-    <mergeCell ref="D58:D63"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="C35:C38"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="B150:B152"/>
-    <mergeCell ref="B145:B149"/>
-    <mergeCell ref="B157:B164"/>
-    <mergeCell ref="B153:B156"/>
-    <mergeCell ref="C8:C12"/>
-    <mergeCell ref="D8:D12"/>
-    <mergeCell ref="D16:D19"/>
-    <mergeCell ref="D170:D177"/>
-    <mergeCell ref="C170:C177"/>
-    <mergeCell ref="C150:C152"/>
-    <mergeCell ref="D150:D152"/>
-    <mergeCell ref="C145:C149"/>
-    <mergeCell ref="D145:D149"/>
-    <mergeCell ref="D157:D164"/>
-    <mergeCell ref="C157:C164"/>
-    <mergeCell ref="D167:D169"/>
-    <mergeCell ref="D153:D156"/>
+    <mergeCell ref="A157:A199"/>
+    <mergeCell ref="B167:B169"/>
+    <mergeCell ref="C167:C169"/>
+    <mergeCell ref="C153:C156"/>
+    <mergeCell ref="D178:D186"/>
+    <mergeCell ref="C178:C186"/>
+    <mergeCell ref="B178:B186"/>
+    <mergeCell ref="D194:D199"/>
+    <mergeCell ref="C194:C199"/>
+    <mergeCell ref="B194:B199"/>
+    <mergeCell ref="D187:D193"/>
+    <mergeCell ref="C187:C193"/>
+    <mergeCell ref="B187:B193"/>
+    <mergeCell ref="A113:A156"/>
+    <mergeCell ref="B114:B121"/>
+    <mergeCell ref="C114:C121"/>
+    <mergeCell ref="A57:A78"/>
+    <mergeCell ref="D87:D94"/>
+    <mergeCell ref="C87:C94"/>
+    <mergeCell ref="B87:B94"/>
+    <mergeCell ref="A79:A112"/>
+    <mergeCell ref="D101:D105"/>
+    <mergeCell ref="C101:C105"/>
+    <mergeCell ref="B101:B105"/>
+    <mergeCell ref="B95:B98"/>
+    <mergeCell ref="D106:D112"/>
+    <mergeCell ref="C106:C112"/>
+    <mergeCell ref="B106:B112"/>
+    <mergeCell ref="D95:D98"/>
+    <mergeCell ref="C58:C63"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="F64:F69"/>
+    <mergeCell ref="D64:D69"/>
+    <mergeCell ref="C64:C69"/>
+    <mergeCell ref="B64:B69"/>
+    <mergeCell ref="D123:D144"/>
+    <mergeCell ref="D70:D78"/>
+    <mergeCell ref="C70:C78"/>
+    <mergeCell ref="B70:B78"/>
+    <mergeCell ref="B123:B144"/>
+    <mergeCell ref="D114:D121"/>
+    <mergeCell ref="C123:C144"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="A27:A56"/>
     <mergeCell ref="D39:D47"/>
@@ -44770,48 +44785,33 @@
     <mergeCell ref="C16:C19"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="A16:A26"/>
-    <mergeCell ref="F64:F69"/>
-    <mergeCell ref="D64:D69"/>
-    <mergeCell ref="C64:C69"/>
-    <mergeCell ref="B64:B69"/>
-    <mergeCell ref="D123:D144"/>
-    <mergeCell ref="D70:D78"/>
-    <mergeCell ref="C70:C78"/>
-    <mergeCell ref="B70:B78"/>
-    <mergeCell ref="B123:B144"/>
-    <mergeCell ref="D114:D121"/>
-    <mergeCell ref="C123:C144"/>
-    <mergeCell ref="A57:A78"/>
-    <mergeCell ref="D87:D94"/>
-    <mergeCell ref="C87:C94"/>
-    <mergeCell ref="B87:B94"/>
-    <mergeCell ref="A79:A112"/>
-    <mergeCell ref="D101:D105"/>
-    <mergeCell ref="C101:C105"/>
-    <mergeCell ref="B101:B105"/>
-    <mergeCell ref="B95:B98"/>
-    <mergeCell ref="D106:D112"/>
-    <mergeCell ref="C106:C112"/>
-    <mergeCell ref="B106:B112"/>
-    <mergeCell ref="D95:D98"/>
-    <mergeCell ref="C58:C63"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="A157:A199"/>
-    <mergeCell ref="B167:B169"/>
-    <mergeCell ref="C167:C169"/>
-    <mergeCell ref="C153:C156"/>
-    <mergeCell ref="D178:D186"/>
-    <mergeCell ref="C178:C186"/>
-    <mergeCell ref="B178:B186"/>
-    <mergeCell ref="D194:D199"/>
-    <mergeCell ref="C194:C199"/>
-    <mergeCell ref="B194:B199"/>
-    <mergeCell ref="D187:D193"/>
-    <mergeCell ref="C187:C193"/>
-    <mergeCell ref="B187:B193"/>
-    <mergeCell ref="A113:A156"/>
-    <mergeCell ref="B114:B121"/>
-    <mergeCell ref="C114:C121"/>
+    <mergeCell ref="C8:C12"/>
+    <mergeCell ref="D8:D12"/>
+    <mergeCell ref="D16:D19"/>
+    <mergeCell ref="D170:D177"/>
+    <mergeCell ref="C170:C177"/>
+    <mergeCell ref="C150:C152"/>
+    <mergeCell ref="D150:D152"/>
+    <mergeCell ref="C145:C149"/>
+    <mergeCell ref="D145:D149"/>
+    <mergeCell ref="D157:D164"/>
+    <mergeCell ref="C157:C164"/>
+    <mergeCell ref="D167:D169"/>
+    <mergeCell ref="D153:D156"/>
+    <mergeCell ref="B170:B177"/>
+    <mergeCell ref="D165:D166"/>
+    <mergeCell ref="C165:C166"/>
+    <mergeCell ref="B165:B166"/>
+    <mergeCell ref="B28:B33"/>
+    <mergeCell ref="C95:C98"/>
+    <mergeCell ref="D58:D63"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="C35:C38"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="B150:B152"/>
+    <mergeCell ref="B145:B149"/>
+    <mergeCell ref="B157:B164"/>
+    <mergeCell ref="B153:B156"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" fitToHeight="4" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>